<commit_message>
Fixed auth tokken not using resi
</commit_message>
<xml_diff>
--- a/PrototypeContexProvider/TestApp/Benchmarks/LoadedInBenchmark.xlsx
+++ b/PrototypeContexProvider/TestApp/Benchmarks/LoadedInBenchmark.xlsx
@@ -1,49 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/64f2fa06baeddabd/Documents/GitHub/PrototypeContextProvider/PrototypeContexProvider/TestApp/Benchmarks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfsar\OneDrive\Documents\GitHub\PrototypeContextProvider\PrototypeContexProvider\TestApp\Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C3E4B2C-5A0D-41F0-A955-EB7C6E12D10D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{8C3E4B2C-5A0D-41F0-A955-EB7C6E12D10D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{E1F7811C-197F-4962-BE0B-9C2A98EAE3FF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28793" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28793" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoadedInBenchmark" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>none</t>
+    <t>three Loaded</t>
   </si>
   <si>
-    <t>one</t>
+    <t>none Unlaoded</t>
   </si>
   <si>
-    <t>two</t>
+    <t>one Unlaoded</t>
   </si>
   <si>
-    <t>three</t>
+    <t>two Unlaoded</t>
+  </si>
+  <si>
+    <t>three Unlaoded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -616,12 +616,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-AU"/>
-              <a:t>Loaded</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> in Benchmark</a:t>
+              <a:t>Benchmark</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -671,7 +667,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>none</c:v>
+                  <c:v>three Loaded</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -716,16 +712,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>1326</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>229</c:v>
+                  <c:v>11264</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -746,7 +742,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>one</c:v>
+                  <c:v>none Unlaoded</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -791,16 +787,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>6514</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>81551</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>257</c:v>
+                  <c:v>1228204</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16211</c:v>
+                  <c:v>5769318</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -821,7 +817,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>two</c:v>
+                  <c:v>one Unlaoded</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -866,16 +862,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>17</c:v>
+                  <c:v>5501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76</c:v>
+                  <c:v>54806</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>607</c:v>
+                  <c:v>541307</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5965</c:v>
+                  <c:v>5344436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -896,7 +892,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>three</c:v>
+                  <c:v>two Unlaoded</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -941,16 +937,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>4899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>133</c:v>
+                  <c:v>61437</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1326</c:v>
+                  <c:v>542242</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11264</c:v>
+                  <c:v>5476202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -959,6 +955,310 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-2D1A-457B-BDA8-74171F6B4CC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LoadedInBenchmark!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>three Unlaoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7725</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>615722</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6228051</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF8B-483A-9B06-ACD989B7CB50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LoadedInBenchmark!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one Unlaoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54806</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>541307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5344436</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF8B-483A-9B06-ACD989B7CB50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LoadedInBenchmark!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>two Unlaoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>542242</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5476202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FF8B-483A-9B06-ACD989B7CB50}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LoadedInBenchmark!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>three Unlaoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$1:$E$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LoadedInBenchmark!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>7725</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>615722</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6228051</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-FF8B-483A-9B06-ACD989B7CB50}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1207,8 +1507,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.26338097826823492"/>
           <c:y val="0.88866306176154242"/>
-          <c:w val="0.54226727909011374"/>
-          <c:h val="7.8125546806649182E-2"/>
+          <c:w val="0.7366189434426379"/>
+          <c:h val="0.1113367599883348"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1839,15 +2139,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>157162</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>178593</xdr:rowOff>
+      <xdr:colOff>157161</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>11906</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>195262</xdr:colOff>
+      <xdr:colOff>500062</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>26193</xdr:rowOff>
+      <xdr:rowOff>40481</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1873,102 +2173,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="UnloadedBenchmark"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1">
-            <v>10</v>
-          </cell>
-          <cell r="C1">
-            <v>100</v>
-          </cell>
-          <cell r="D1">
-            <v>1000</v>
-          </cell>
-          <cell r="E1">
-            <v>10000</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>none</v>
-          </cell>
-          <cell r="B2">
-            <v>6514</v>
-          </cell>
-          <cell r="C2">
-            <v>81551</v>
-          </cell>
-          <cell r="D2">
-            <v>1228204</v>
-          </cell>
-          <cell r="E2">
-            <v>5769318</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>one</v>
-          </cell>
-          <cell r="B3">
-            <v>5501</v>
-          </cell>
-          <cell r="C3">
-            <v>54806</v>
-          </cell>
-          <cell r="D3">
-            <v>541307</v>
-          </cell>
-          <cell r="E3">
-            <v>5344436</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>two</v>
-          </cell>
-          <cell r="B4">
-            <v>4899</v>
-          </cell>
-          <cell r="C4">
-            <v>61437</v>
-          </cell>
-          <cell r="D4">
-            <v>542242</v>
-          </cell>
-          <cell r="E4">
-            <v>5476202</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>three</v>
-          </cell>
-          <cell r="B5">
-            <v>7725</v>
-          </cell>
-          <cell r="C5">
-            <v>59505</v>
-          </cell>
-          <cell r="D5">
-            <v>615722</v>
-          </cell>
-          <cell r="E5">
-            <v>6228051</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2553,14 +2757,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.46484375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
@@ -2584,16 +2791,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>133</v>
       </c>
       <c r="D2">
-        <v>23</v>
+        <v>1326</v>
       </c>
       <c r="E2">
-        <v>229</v>
+        <v>11264</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
@@ -2601,16 +2808,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>6514</v>
       </c>
       <c r="C3">
-        <v>34</v>
+        <v>81551</v>
       </c>
       <c r="D3">
-        <v>257</v>
+        <v>1228204</v>
       </c>
       <c r="E3">
-        <v>16211</v>
+        <v>5769318</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -2618,16 +2825,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>5501</v>
       </c>
       <c r="C4">
-        <v>76</v>
+        <v>54806</v>
       </c>
       <c r="D4">
-        <v>607</v>
+        <v>541307</v>
       </c>
       <c r="E4">
-        <v>5965</v>
+        <v>5344436</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -2635,16 +2842,84 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>19</v>
+        <v>4899</v>
       </c>
       <c r="C5">
-        <v>133</v>
+        <v>61437</v>
       </c>
       <c r="D5">
-        <v>1326</v>
+        <v>542242</v>
       </c>
       <c r="E5">
-        <v>11264</v>
+        <v>5476202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>7725</v>
+      </c>
+      <c r="C6">
+        <v>59505</v>
+      </c>
+      <c r="D6">
+        <v>615722</v>
+      </c>
+      <c r="E6">
+        <v>6228051</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>5501</v>
+      </c>
+      <c r="C7">
+        <v>54806</v>
+      </c>
+      <c r="D7">
+        <v>541307</v>
+      </c>
+      <c r="E7">
+        <v>5344436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>4899</v>
+      </c>
+      <c r="C8">
+        <v>61437</v>
+      </c>
+      <c r="D8">
+        <v>542242</v>
+      </c>
+      <c r="E8">
+        <v>5476202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>7725</v>
+      </c>
+      <c r="C9">
+        <v>59505</v>
+      </c>
+      <c r="D9">
+        <v>615722</v>
+      </c>
+      <c r="E9">
+        <v>6228051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>